<commit_message>
add UseCaseScan, add Bank example
</commit_message>
<xml_diff>
--- a/Reports/Report1/UseCaseVorlage.xlsx
+++ b/Reports/Report1/UseCaseVorlage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Number</t>
   </si>
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,21 +101,13 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -132,7 +124,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -148,17 +140,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -187,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,19 +181,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,151 +270,185 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B8:G25"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.8520408163265"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="77.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.1581632653061"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="5"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>